<commit_message>
Added Products to home page and sorted the menu list.
</commit_message>
<xml_diff>
--- a/LEIK - Catálogo Web.xlsx
+++ b/LEIK - Catálogo Web.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC1\PycharmProjects\LeikWebSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C25AD4-EEE6-4231-9490-4617004738BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F4E72C-8FF9-4039-A7A3-0769B64AE815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catálogo - Productos" sheetId="1" r:id="rId1"/>
-    <sheet name="Bases" sheetId="30" r:id="rId2"/>
-    <sheet name="Brochas" sheetId="31" r:id="rId3"/>
-    <sheet name="Corporales" sheetId="32" r:id="rId4"/>
-    <sheet name="Correctores" sheetId="33" r:id="rId5"/>
-    <sheet name="Delineadores" sheetId="34" r:id="rId6"/>
-    <sheet name="Esponjitas" sheetId="35" r:id="rId7"/>
-    <sheet name="Labiales" sheetId="36" r:id="rId8"/>
-    <sheet name="Otros" sheetId="37" r:id="rId9"/>
-    <sheet name="Paletas" sheetId="38" r:id="rId10"/>
-    <sheet name="Pestañinas" sheetId="39" r:id="rId11"/>
-    <sheet name="Polvos" sheetId="40" r:id="rId12"/>
-    <sheet name="Primer" sheetId="41" r:id="rId13"/>
-    <sheet name="Rubores" sheetId="42" r:id="rId14"/>
-    <sheet name="Sombras" sheetId="43" r:id="rId15"/>
+    <sheet name="Productos" sheetId="44" r:id="rId2"/>
+    <sheet name="Bases" sheetId="30" r:id="rId3"/>
+    <sheet name="Brochas" sheetId="31" r:id="rId4"/>
+    <sheet name="Corporales" sheetId="32" r:id="rId5"/>
+    <sheet name="Correctores" sheetId="33" r:id="rId6"/>
+    <sheet name="Delineadores" sheetId="34" r:id="rId7"/>
+    <sheet name="Esponjitas" sheetId="35" r:id="rId8"/>
+    <sheet name="Labiales" sheetId="36" r:id="rId9"/>
+    <sheet name="Otros" sheetId="37" r:id="rId10"/>
+    <sheet name="Paletas" sheetId="38" r:id="rId11"/>
+    <sheet name="Pestañinas" sheetId="39" r:id="rId12"/>
+    <sheet name="Polvos" sheetId="40" r:id="rId13"/>
+    <sheet name="Primer" sheetId="41" r:id="rId14"/>
+    <sheet name="Rubores" sheetId="42" r:id="rId15"/>
+    <sheet name="Sombras" sheetId="43" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catálogo - Productos'!$A$1:$F$156</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="542">
   <si>
     <t>Categoría</t>
   </si>
@@ -2031,6 +2032,15 @@
   </si>
   <si>
     <t>NoDisponible.png</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Iconos</t>
+  </si>
+  <si>
+    <t>book</t>
   </si>
 </sst>
 </file>
@@ -2213,7 +2223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2266,6 +2276,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2657,7 +2668,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -2725,7 +2736,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -3091,9 +3102,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7857,6 +7868,323 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B3C1CD-4C75-47D9-A928-5953E9A36640}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="27">
+        <v>26086.959999999999</v>
+      </c>
+      <c r="G2" s="27">
+        <v>23478.26</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="27">
+        <v>18843.39</v>
+      </c>
+      <c r="G3" s="27">
+        <v>16959.05</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="27">
+        <v>9688.35</v>
+      </c>
+      <c r="G4" s="27">
+        <v>8719.51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="27">
+        <v>35294.120000000003</v>
+      </c>
+      <c r="G5" s="27">
+        <v>31764.71</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="27">
+        <v>17730.5</v>
+      </c>
+      <c r="G6" s="27">
+        <v>15957.45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="27">
+        <v>3546.1</v>
+      </c>
+      <c r="G7" s="27">
+        <v>3191.49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="27">
+        <v>13317.76</v>
+      </c>
+      <c r="G8" s="27">
+        <v>11985.98</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="I8" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="27">
+        <v>24000</v>
+      </c>
+      <c r="G9" s="27">
+        <v>21600</v>
+      </c>
+      <c r="I9" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="27">
+        <v>24000</v>
+      </c>
+      <c r="G10" s="27">
+        <v>21600</v>
+      </c>
+      <c r="I10" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="27">
+        <v>12000</v>
+      </c>
+      <c r="G11" s="27">
+        <v>10800</v>
+      </c>
+      <c r="I11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E43DF8B-B353-4AF2-97C0-E8881076D603}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -8188,7 +8516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5228FCD-D6D0-43D6-8288-D5ABE34D31D6}">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -9116,7 +9444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04074722-15F8-4D43-9F7E-95ACB5C52E05}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -9413,7 +9741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFD1939-76B2-4988-9AF5-0F19C6946788}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -9571,7 +9899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7B64EF-0BBC-4487-AB3B-052532EAE34C}">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -10157,7 +10485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B139D3-C392-4C0E-A8BA-4CB1552B5CF8}">
   <dimension ref="A1:I15"/>
   <sheetViews>
@@ -10585,6 +10913,147 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF52C765-DB32-4675-A1D8-2D90ACBF5347}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>539</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B12" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B13" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>352</v>
+      </c>
+      <c r="B14" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>400</v>
+      </c>
+      <c r="B15" t="s">
+        <v>541</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD0BD2A-B12B-49B4-A0AB-5B1EBFA6D2CF}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -10742,13 +11211,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4A55FE-FCF6-4CC0-9BA8-207E1362E1E4}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -11259,7 +11733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FDF7A8-B649-4698-88F8-5CC9B8392A34}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -11359,7 +11833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FF65BF-4039-4A89-8D45-9C0911433869}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -11572,7 +12046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B8AE7B-ABBC-480A-A24F-9F080C1F0B2D}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -11898,7 +12372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B77EF1-97FE-47C7-84ED-0B8C5CAC85A0}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -12105,7 +12579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F773F2-CF84-4589-A297-44FDD6F2963F}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -12461,321 +12935,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B3C1CD-4C75-47D9-A928-5953E9A36640}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="27">
-        <v>26086.959999999999</v>
-      </c>
-      <c r="G2" s="27">
-        <v>23478.26</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="I2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="27">
-        <v>18843.39</v>
-      </c>
-      <c r="G3" s="27">
-        <v>16959.05</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="I3" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="27">
-        <v>9688.35</v>
-      </c>
-      <c r="G4" s="27">
-        <v>8719.51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="27">
-        <v>35294.120000000003</v>
-      </c>
-      <c r="G5" s="27">
-        <v>31764.71</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="I5" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="27">
-        <v>17730.5</v>
-      </c>
-      <c r="G6" s="27">
-        <v>15957.45</v>
-      </c>
-      <c r="I6" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="27">
-        <v>3546.1</v>
-      </c>
-      <c r="G7" s="27">
-        <v>3191.49</v>
-      </c>
-      <c r="I7" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="27">
-        <v>13317.76</v>
-      </c>
-      <c r="G8" s="27">
-        <v>11985.98</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="I8" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="27">
-        <v>24000</v>
-      </c>
-      <c r="G9" s="27">
-        <v>21600</v>
-      </c>
-      <c r="I9" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="27">
-        <v>24000</v>
-      </c>
-      <c r="G10" s="27">
-        <v>21600</v>
-      </c>
-      <c r="I10" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="27">
-        <v>12000</v>
-      </c>
-      <c r="G11" s="27">
-        <v>10800</v>
-      </c>
-      <c r="I11" t="s">
-        <v>538</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-structured the items in 4 columns and the code was improved for each item in a function called structure
</commit_message>
<xml_diff>
--- a/LEIK - Catálogo Web.xlsx
+++ b/LEIK - Catálogo Web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC1\PycharmProjects\LeikWebSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F4E72C-8FF9-4039-A7A3-0769B64AE815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E976334-E499-49EC-BDE3-BB2AE0DE3FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catálogo - Productos" sheetId="1" r:id="rId1"/>
@@ -7871,9 +7871,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B3C1CD-4C75-47D9-A928-5953E9A36640}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -9906,6 +9913,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10917,7 +10929,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>